<commit_message>
changes to region contignecy table
</commit_message>
<xml_diff>
--- a/EcologyBiasTables.xlsx
+++ b/EcologyBiasTables.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/veronicamarquez/Desktop/Dr.D Ecology Bias SC/MA321-Daneshgar/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8653DB4-49C9-774D-99CA-83F895E7BFBB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="89">
   <si>
     <t>Ecosystem</t>
   </si>
@@ -297,12 +296,15 @@
   </si>
   <si>
     <t>Mid-South</t>
+  </si>
+  <si>
+    <t>South Atlantic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -358,99 +360,99 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Ecosystem" displayName="Ecosystem" ref="A1:B4" totalsRowShown="0">
-  <autoFilter ref="A1:B4" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Ecosystem" displayName="Ecosystem" ref="A1:B4" totalsRowShown="0">
+  <autoFilter ref="A1:B4"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Ecosystem"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Counts"/>
+    <tableColumn id="1" name="Ecosystem"/>
+    <tableColumn id="2" name="Counts"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Region" displayName="Region" ref="D1:E10" totalsRowShown="0">
-  <autoFilter ref="D1:E10" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Region" displayName="Region" ref="D1:E10" totalsRowShown="0">
+  <autoFilter ref="D1:E10"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Region"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Count"/>
+    <tableColumn id="1" name="Region"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Continents" displayName="Continents" ref="G1:H8" totalsRowShown="0">
-  <autoFilter ref="G1:H8" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Continents" displayName="Continents" ref="G1:H8" totalsRowShown="0">
+  <autoFilter ref="G1:H8"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Continent"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Count"/>
+    <tableColumn id="1" name="Continent"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Countries" displayName="Countries" ref="A14:B50" totalsRowShown="0">
-  <autoFilter ref="A14:B50" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Countries" displayName="Countries" ref="A14:B50" totalsRowShown="0">
+  <autoFilter ref="A14:B50"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Country"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Count"/>
+    <tableColumn id="1" name="Country"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="States" displayName="States" ref="D15:E41" totalsRowShown="0">
-  <autoFilter ref="D15:E41" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="States" displayName="States" ref="D15:E41" totalsRowShown="0">
+  <autoFilter ref="D15:E41"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="State"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Count"/>
+    <tableColumn id="1" name="State"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{55B14A11-A330-B04C-952A-9E9AC5070762}" name="Countries9" displayName="Countries9" ref="A1:B37" totalsRowShown="0">
-  <autoFilter ref="A1:B37" xr:uid="{BFC2068E-0B73-6F45-9D5E-F3A0A579C040}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Countries9" displayName="Countries9" ref="A1:B37" totalsRowShown="0">
+  <autoFilter ref="A1:B37"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A0467016-DE61-1A45-A691-A8F30524C01B}" name="Country"/>
-    <tableColumn id="2" xr3:uid="{B0AD24A3-BA15-9947-9C42-5ED3DE8835A8}" name="Count"/>
+    <tableColumn id="1" name="Country"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{76B78CA8-E4E4-F14B-9340-D4AD390B549F}" name="Region3" displayName="Region3" ref="A1:B11" totalsRowShown="0">
-  <autoFilter ref="A1:B11" xr:uid="{9CE0DC42-1C59-294B-A89A-A68D41522C01}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Region3" displayName="Region3" ref="A1:B11" totalsRowShown="0">
+  <autoFilter ref="A1:B11"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F94CA18F-BC33-8240-81C7-88644CC94E1B}" name="Region"/>
-    <tableColumn id="2" xr3:uid="{F00A52D0-070F-194F-A4BC-1B37C6D88EAA}" name="Count"/>
+    <tableColumn id="1" name="Region"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D234AC4D-0F58-7B47-907D-494F6594F1F7}" name="Continents8" displayName="Continents8" ref="A1:B8" totalsRowShown="0">
-  <autoFilter ref="A1:B8" xr:uid="{A5DFB51F-3F68-504F-BB28-E938D2967D38}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Continents8" displayName="Continents8" ref="A1:B8" totalsRowShown="0">
+  <autoFilter ref="A1:B8"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6B7E53CF-5465-C346-9057-3576148B8B12}" name="Continent"/>
-    <tableColumn id="2" xr3:uid="{58DF6188-128F-6344-9E3D-47220AB9C42F}" name="Count"/>
+    <tableColumn id="1" name="Continent"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9EE74738-A42C-1E4F-A9B5-3EFA8F44640B}" name="States10" displayName="States10" ref="A1:B27" totalsRowShown="0">
-  <autoFilter ref="A1:B27" xr:uid="{B48134A9-DD3B-C445-9F25-6915C4ADAC05}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="States10" displayName="States10" ref="A1:B27" totalsRowShown="0">
+  <autoFilter ref="A1:B27"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{6D83F8FC-4D75-7448-9C2F-A3A638881514}" name="State"/>
-    <tableColumn id="2" xr3:uid="{78271576-48D1-3C45-9F87-AB55724A042B}" name="Count"/>
+    <tableColumn id="1" name="State"/>
+    <tableColumn id="2" name="Count"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -718,13 +720,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A34" workbookViewId="0">
       <selection activeCell="D15" sqref="D15:E41"/>
     </sheetView>
   </sheetViews>
@@ -1363,7 +1365,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9D5E316-0F81-FC48-B2F3-179F81A5984A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1677,7 +1679,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6E25248-53A0-2442-8ADE-A18FACBF7FF3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1689,11 +1691,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8D706D-3378-0D4C-A42C-B2B31360E023}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="267" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A9" sqref="A9:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1767,7 +1769,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>88</v>
       </c>
       <c r="B9">
         <v>10</v>
@@ -1798,7 +1800,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EA1A4A8-566E-854D-8AEC-8D404D99768A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1880,7 +1882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B54061D-A409-CC4F-A39C-6FE6ADF441F6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView topLeftCell="A193" workbookViewId="0">

</xml_diff>